<commit_message>
FIDCARE, Aggiunta sezione entryRelationShip
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111KIRANETXXXX/KIRANET/FIDCARE/5.4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111KIRANETXXXX/KIRANET/FIDCARE/5.4.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.schiavottiello\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.schiavottiello\Desktop\Accreditamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D8591B-C42A-41D7-8B83-535D677E6EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B24CA06-020C-4AC2-9416-C584FF747A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -977,22 +977,22 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>2023-06-01T16:31:48Z</t>
-  </si>
-  <si>
-    <t>bdcc3947398373bf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.ac776f6706f46ca2bf7800d5dfd9c70308e9a74ff4f6f3130dcc0a1a3a8e1916.d539f92de4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>3e4ad0b1dd287f35</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.ac776f6706f46ca2bf7800d5dfd9c70308e9a74ff4f6f3130dcc0a1a3a8e1916.fd6bb84797^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-01T17:36:55Z</t>
+    <t>2023-06-05T22:11:34Z</t>
+  </si>
+  <si>
+    <t>76d2de0afe23dd99</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.ac776f6706f46ca2bf7800d5dfd9c70308e9a74ff4f6f3130dcc0a1a3a8e1916.09719d747e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-05T22:19:42Z</t>
+  </si>
+  <si>
+    <t>be4959b4562b9737</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.ac776f6706f46ca2bf7800d5dfd9c70308e9a74ff4f6f3130dcc0a1a3a8e1916.c1074dee7c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3177,8 +3177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T653"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3606,7 +3606,7 @@
         <v>65</v>
       </c>
       <c r="F13" s="37">
-        <v>45078</v>
+        <v>45082</v>
       </c>
       <c r="G13" s="38" t="s">
         <v>187</v>
@@ -4036,16 +4036,16 @@
         <v>96</v>
       </c>
       <c r="F24" s="37">
-        <v>45078</v>
+        <v>45082</v>
       </c>
       <c r="G24" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="H24" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="I24" s="38" t="s">
         <v>192</v>
-      </c>
-      <c r="H24" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="I24" s="38" t="s">
-        <v>191</v>
       </c>
       <c r="J24" s="40" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Valorizzazione colonne O e P per i test 32 e 40
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111KIRANETXXXX/KIRANET/FIDCARE/5.4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111KIRANETXXXX/KIRANET/FIDCARE/5.4.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.schiavottiello\Desktop\Accreditamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.schiavottiello\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF692ABA-B41E-43F4-A389-7E7829A44108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECFC3DB-0C4E-4C42-BAF1-E97D6DAD31FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="194">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -993,6 +993,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.ac776f6706f46ca2bf7800d5dfd9c70308e9a74ff4f6f3130dcc0a1a3a8e1916.c1074dee7c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Gestito come bug da risolvere</t>
   </si>
 </sst>
 </file>
@@ -3177,8 +3180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T653"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3486,8 +3489,12 @@
       <c r="N10" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
+      <c r="O10" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="P10" s="41" t="s">
+        <v>193</v>
+      </c>
       <c r="Q10" s="40" t="s">
         <v>55</v>
       </c>
@@ -3536,8 +3543,12 @@
       <c r="N11" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
+      <c r="O11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="P11" s="41" t="s">
+        <v>193</v>
+      </c>
       <c r="Q11" s="40" t="s">
         <v>55</v>
       </c>
@@ -18112,7 +18123,7 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J12:J14 L12:M14 O12 O14:O20 J15:J19 L15:M24 J21:J35 O21:O35 L28:M35" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O12 J12:J19 L12:M24 J21:J35 O14:O35 L28:M35" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q12:Q35" xr:uid="{00000000-0002-0000-0200-000001000000}">

</xml_diff>

<commit_message>
Colonna applicabilità test id 48
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111KIRANETXXXX/KIRANET/FIDCARE/5.4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111KIRANETXXXX/KIRANET/FIDCARE/5.4.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.schiavottiello\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECFC3DB-0C4E-4C42-BAF1-E97D6DAD31FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B58093-F6F7-45F3-9270-9E194730D31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="194">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3180,8 +3180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T653"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3578,7 +3578,9 @@
       <c r="G12" s="39"/>
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
-      <c r="J12" s="41"/>
+      <c r="J12" s="41" t="s">
+        <v>63</v>
+      </c>
       <c r="K12" s="41"/>
       <c r="L12" s="40" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Dettaglio gestione casi 32, 40 e 48
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111KIRANETXXXX/KIRANET/FIDCARE/5.4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111KIRANETXXXX/KIRANET/FIDCARE/5.4.0/report-checklist.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.schiavottiello\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.caterino\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B58093-F6F7-45F3-9270-9E194730D31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -24,12 +23,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autore importato</author>
   </authors>
   <commentList>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="E9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="196">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -995,17 +994,23 @@
     <t>2.16.840.1.113883.2.9.2.150.4.4.ac776f6706f46ca2bf7800d5dfd9c70308e9a74ff4f6f3130dcc0a1a3a8e1916.c1074dee7c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Gestito come bug da risolvere</t>
+    <t>Mostrato a video l'errore evidenziato "Richiesta validazione non avvenuta", l'utente contatta l'assistenza che prova a correggere l'errore visualizzando i log dell'applicativo ed eventualmente gli chiede di validare nuovamente</t>
+  </si>
+  <si>
+    <t>Timeout di Connessione.</t>
+  </si>
+  <si>
+    <t>Mostrato a video l'errore "Timeout di connessione", l'utente contatta l'assistenza che prova a correggere l'errore visualizzando i log dell'applicativo ed eventualmente gli chiede di validare nuovamente.Nel caso in cui non sia possibile validare,il processo clinico prosegue e il documento viene salvato e risottomesso alla validazione al ripristinarsi del servizio attraverso uno script dell'applicativo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-m\-d"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1052,6 +1057,12 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1079,7 +1090,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1557,6 +1568,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
@@ -1671,7 +1695,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1754,6 +1777,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2884,7 +2910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -3018,7 +3044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -3177,11 +3203,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T653"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3225,12 +3251,12 @@
       <c r="T1" s="23"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="75"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74"/>
       <c r="E2" s="13"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
@@ -3249,14 +3275,14 @@
       <c r="T2" s="23"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="82" t="s">
+      <c r="B3" s="76"/>
+      <c r="C3" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="75"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="13"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
@@ -3275,12 +3301,12 @@
       <c r="T3" s="23"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="78"/>
-      <c r="B4" s="79"/>
-      <c r="C4" s="82" t="s">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="75"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="13"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
@@ -3299,12 +3325,12 @@
       <c r="T4" s="23"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="80"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="82" t="s">
+      <c r="A5" s="79"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="75"/>
+      <c r="D5" s="74"/>
       <c r="E5" s="13"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
@@ -3323,8 +3349,8 @@
       <c r="T5" s="23"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="70"/>
-      <c r="B6" s="71"/>
+      <c r="A6" s="69"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="24"/>
       <c r="D6" s="25"/>
       <c r="E6" s="3"/>
@@ -3388,7 +3414,7 @@
       <c r="S8" s="30"/>
       <c r="T8" s="31"/>
     </row>
-    <row r="9" spans="1:20" ht="14.25" customHeight="1">
+    <row r="9" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
       <c r="A9" s="32" t="s">
         <v>27</v>
       </c>
@@ -3450,7 +3476,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="129.6" customHeight="1">
+    <row r="10" spans="1:20" ht="129.6" customHeight="1" thickBot="1">
       <c r="A10" s="34">
         <v>32</v>
       </c>
@@ -3490,9 +3516,9 @@
         <v>54</v>
       </c>
       <c r="O10" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="P10" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="P10" s="82" t="s">
         <v>193</v>
       </c>
       <c r="Q10" s="40" t="s">
@@ -3504,7 +3530,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="144" customHeight="1">
+    <row r="11" spans="1:20" ht="144" customHeight="1" thickBot="1">
       <c r="A11" s="34">
         <v>40</v>
       </c>
@@ -3544,9 +3570,9 @@
         <v>54</v>
       </c>
       <c r="O11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="P11" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="P11" s="82" t="s">
         <v>193</v>
       </c>
       <c r="Q11" s="40" t="s">
@@ -3588,10 +3614,14 @@
       <c r="M12" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="N12" s="45"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="40" t="s">
-        <v>54</v>
+      <c r="N12" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="O12" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="P12" s="82" t="s">
+        <v>195</v>
       </c>
       <c r="Q12" s="40" t="s">
         <v>55</v>
@@ -4481,40 +4511,40 @@
       </c>
     </row>
     <row r="35" spans="1:20" ht="115.2" customHeight="1">
-      <c r="A35" s="46">
+      <c r="A35" s="45">
         <v>169</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="47" t="s">
+      <c r="D35" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="E35" s="48" t="s">
+      <c r="E35" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="50" t="s">
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="K35" s="50" t="s">
+      <c r="K35" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="L35" s="51"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="51"/>
-      <c r="O35" s="51"/>
-      <c r="P35" s="51"/>
-      <c r="Q35" s="51"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="52"/>
-      <c r="T35" s="53" t="s">
+      <c r="L35" s="50"/>
+      <c r="M35" s="50"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="50"/>
+      <c r="P35" s="50"/>
+      <c r="Q35" s="50"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="51"/>
+      <c r="T35" s="52" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4524,21 +4554,21 @@
       <c r="C36" s="25"/>
       <c r="D36" s="25"/>
       <c r="E36" s="25"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="55"/>
-      <c r="R36" s="56"/>
-      <c r="S36" s="57"/>
-      <c r="T36" s="58"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="54"/>
+      <c r="N36" s="54"/>
+      <c r="O36" s="54"/>
+      <c r="P36" s="54"/>
+      <c r="Q36" s="54"/>
+      <c r="R36" s="55"/>
+      <c r="S36" s="56"/>
+      <c r="T36" s="57"/>
     </row>
     <row r="37" spans="1:20" ht="14.25" customHeight="1">
       <c r="A37" s="3"/>
@@ -18125,10 +18155,10 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O12 J12:J19 L12:M24 J21:J35 O14:O35 L28:M35" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O12 J12:J19 L12:M24 J21:J35 O14:O35 L28:M35">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q12:Q35" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q12:Q35">
       <formula1>"PASS,FAIL"</formula1>
     </dataValidation>
   </dataValidations>
@@ -18142,7 +18172,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -18159,16 +18189,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="58" t="s">
         <v>130</v>
       </c>
       <c r="E1" s="13"/>
@@ -18180,10 +18210,10 @@
       <c r="B2" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="59" t="s">
         <v>134</v>
       </c>
       <c r="E2" s="13"/>
@@ -18195,10 +18225,10 @@
       <c r="B3" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="59" t="s">
         <v>137</v>
       </c>
       <c r="E3" s="13"/>
@@ -18210,10 +18240,10 @@
       <c r="B4" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="60" t="s">
         <v>140</v>
       </c>
       <c r="E4" s="13"/>
@@ -18225,10 +18255,10 @@
       <c r="B5" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="59" t="s">
         <v>143</v>
       </c>
       <c r="E5" s="13"/>
@@ -18240,10 +18270,10 @@
       <c r="B6" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="60" t="s">
         <v>146</v>
       </c>
       <c r="E6" s="13"/>
@@ -18255,10 +18285,10 @@
       <c r="B7" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="60" t="s">
         <v>149</v>
       </c>
       <c r="E7" s="13"/>
@@ -18270,10 +18300,10 @@
       <c r="B8" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="60" t="s">
         <v>151</v>
       </c>
       <c r="E8" s="13"/>
@@ -18285,10 +18315,10 @@
       <c r="B9" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="59" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="60" t="s">
         <v>154</v>
       </c>
       <c r="E9" s="13"/>
@@ -18300,10 +18330,10 @@
       <c r="B10" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C10" s="62">
+      <c r="C10" s="61">
         <v>191</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="59" t="s">
         <v>156</v>
       </c>
       <c r="E10" s="13"/>
@@ -18315,10 +18345,10 @@
       <c r="B11" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C11" s="62">
+      <c r="C11" s="61">
         <v>192</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="59" t="s">
         <v>158</v>
       </c>
       <c r="E11" s="13"/>
@@ -18330,10 +18360,10 @@
       <c r="B12" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="62">
+      <c r="C12" s="61">
         <v>208</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="59" t="s">
         <v>159</v>
       </c>
       <c r="E12" s="13"/>
@@ -18345,10 +18375,10 @@
       <c r="B13" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C13" s="62">
+      <c r="C13" s="61">
         <v>224</v>
       </c>
-      <c r="D13" s="61" t="s">
+      <c r="D13" s="60" t="s">
         <v>160</v>
       </c>
       <c r="E13" s="13"/>
@@ -18360,10 +18390,10 @@
       <c r="B14" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C14" s="62">
+      <c r="C14" s="61">
         <v>240</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="59" t="s">
         <v>161</v>
       </c>
       <c r="E14" s="13"/>
@@ -18375,10 +18405,10 @@
       <c r="B15" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C15" s="62">
+      <c r="C15" s="61">
         <v>256</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="60" t="s">
         <v>162</v>
       </c>
       <c r="E15" s="13"/>
@@ -18390,10 +18420,10 @@
       <c r="B16" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="62">
+      <c r="C16" s="61">
         <v>272</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="60" t="s">
         <v>163</v>
       </c>
       <c r="E16" s="13"/>
@@ -18405,10 +18435,10 @@
       <c r="B17" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C17" s="62">
+      <c r="C17" s="61">
         <v>288</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="60" t="s">
         <v>164</v>
       </c>
       <c r="E17" s="13"/>
@@ -18420,10 +18450,10 @@
       <c r="B18" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="62">
+      <c r="C18" s="61">
         <v>304</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="60" t="s">
         <v>165</v>
       </c>
       <c r="E18" s="13"/>
@@ -18435,10 +18465,10 @@
       <c r="B19" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C19" s="62">
+      <c r="C19" s="61">
         <v>193</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="59" t="s">
         <v>167</v>
       </c>
       <c r="E19" s="13"/>
@@ -18450,10 +18480,10 @@
       <c r="B20" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C20" s="62">
+      <c r="C20" s="61">
         <v>209</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="59" t="s">
         <v>168</v>
       </c>
       <c r="E20" s="13"/>
@@ -18465,10 +18495,10 @@
       <c r="B21" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C21" s="62">
+      <c r="C21" s="61">
         <v>225</v>
       </c>
-      <c r="D21" s="61" t="s">
+      <c r="D21" s="60" t="s">
         <v>169</v>
       </c>
       <c r="E21" s="13"/>
@@ -18480,10 +18510,10 @@
       <c r="B22" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C22" s="62">
+      <c r="C22" s="61">
         <v>241</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="59" t="s">
         <v>170</v>
       </c>
       <c r="E22" s="13"/>
@@ -18495,10 +18525,10 @@
       <c r="B23" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C23" s="62">
+      <c r="C23" s="61">
         <v>257</v>
       </c>
-      <c r="D23" s="61" t="s">
+      <c r="D23" s="60" t="s">
         <v>171</v>
       </c>
       <c r="E23" s="13"/>
@@ -18510,10 +18540,10 @@
       <c r="B24" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C24" s="62">
+      <c r="C24" s="61">
         <v>273</v>
       </c>
-      <c r="D24" s="61" t="s">
+      <c r="D24" s="60" t="s">
         <v>172</v>
       </c>
       <c r="E24" s="13"/>
@@ -18525,10 +18555,10 @@
       <c r="B25" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="61">
         <v>289</v>
       </c>
-      <c r="D25" s="61" t="s">
+      <c r="D25" s="60" t="s">
         <v>173</v>
       </c>
       <c r="E25" s="13"/>
@@ -18540,10 +18570,10 @@
       <c r="B26" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C26" s="62">
+      <c r="C26" s="61">
         <v>305</v>
       </c>
-      <c r="D26" s="61" t="s">
+      <c r="D26" s="60" t="s">
         <v>174</v>
       </c>
       <c r="E26" s="13"/>
@@ -18555,10 +18585,10 @@
       <c r="B27" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="62">
+      <c r="C27" s="61">
         <v>194</v>
       </c>
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="59" t="s">
         <v>176</v>
       </c>
       <c r="E27" s="13"/>
@@ -18570,10 +18600,10 @@
       <c r="B28" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C28" s="62">
+      <c r="C28" s="61">
         <v>210</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="59" t="s">
         <v>177</v>
       </c>
       <c r="E28" s="13"/>
@@ -18585,10 +18615,10 @@
       <c r="B29" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C29" s="62">
+      <c r="C29" s="61">
         <v>226</v>
       </c>
-      <c r="D29" s="61" t="s">
+      <c r="D29" s="60" t="s">
         <v>178</v>
       </c>
       <c r="E29" s="13"/>
@@ -18600,10 +18630,10 @@
       <c r="B30" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C30" s="62">
+      <c r="C30" s="61">
         <v>242</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="59" t="s">
         <v>179</v>
       </c>
       <c r="E30" s="13"/>
@@ -18615,10 +18645,10 @@
       <c r="B31" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="62">
+      <c r="C31" s="61">
         <v>258</v>
       </c>
-      <c r="D31" s="61" t="s">
+      <c r="D31" s="60" t="s">
         <v>180</v>
       </c>
       <c r="E31" s="13"/>
@@ -18630,10 +18660,10 @@
       <c r="B32" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C32" s="62">
+      <c r="C32" s="61">
         <v>274</v>
       </c>
-      <c r="D32" s="61" t="s">
+      <c r="D32" s="60" t="s">
         <v>181</v>
       </c>
       <c r="E32" s="13"/>
@@ -18645,10 +18675,10 @@
       <c r="B33" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C33" s="62">
+      <c r="C33" s="61">
         <v>290</v>
       </c>
-      <c r="D33" s="61" t="s">
+      <c r="D33" s="60" t="s">
         <v>182</v>
       </c>
       <c r="E33" s="13"/>
@@ -18660,10 +18690,10 @@
       <c r="B34" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C34" s="62">
+      <c r="C34" s="61">
         <v>306</v>
       </c>
-      <c r="D34" s="61" t="s">
+      <c r="D34" s="60" t="s">
         <v>183</v>
       </c>
       <c r="E34" s="13"/>
@@ -18675,10 +18705,10 @@
       <c r="B35" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C35" s="62">
+      <c r="C35" s="61">
         <v>195</v>
       </c>
-      <c r="D35" s="62">
+      <c r="D35" s="61">
         <v>204</v>
       </c>
       <c r="E35" s="13"/>
@@ -18690,10 +18720,10 @@
       <c r="B36" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C36" s="62">
+      <c r="C36" s="61">
         <v>211</v>
       </c>
-      <c r="D36" s="62">
+      <c r="D36" s="61">
         <v>220</v>
       </c>
       <c r="E36" s="13"/>
@@ -18705,10 +18735,10 @@
       <c r="B37" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C37" s="62">
+      <c r="C37" s="61">
         <v>227</v>
       </c>
-      <c r="D37" s="63">
+      <c r="D37" s="62">
         <v>236</v>
       </c>
       <c r="E37" s="13"/>
@@ -18720,10 +18750,10 @@
       <c r="B38" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C38" s="62">
+      <c r="C38" s="61">
         <v>243</v>
       </c>
-      <c r="D38" s="62">
+      <c r="D38" s="61">
         <v>252</v>
       </c>
       <c r="E38" s="13"/>
@@ -18735,10 +18765,10 @@
       <c r="B39" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C39" s="62">
+      <c r="C39" s="61">
         <v>259</v>
       </c>
-      <c r="D39" s="63">
+      <c r="D39" s="62">
         <v>268</v>
       </c>
       <c r="E39" s="13"/>
@@ -18750,10 +18780,10 @@
       <c r="B40" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C40" s="62">
+      <c r="C40" s="61">
         <v>275</v>
       </c>
-      <c r="D40" s="63">
+      <c r="D40" s="62">
         <v>284</v>
       </c>
       <c r="E40" s="13"/>
@@ -18765,10 +18795,10 @@
       <c r="B41" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C41" s="62">
+      <c r="C41" s="61">
         <v>291</v>
       </c>
-      <c r="D41" s="63">
+      <c r="D41" s="62">
         <v>300</v>
       </c>
       <c r="E41" s="13"/>
@@ -18780,10 +18810,10 @@
       <c r="B42" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C42" s="62">
+      <c r="C42" s="61">
         <v>307</v>
       </c>
-      <c r="D42" s="63">
+      <c r="D42" s="62">
         <v>316</v>
       </c>
       <c r="E42" s="13"/>
@@ -18795,10 +18825,10 @@
       <c r="B43" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C43" s="62">
+      <c r="C43" s="61">
         <v>196</v>
       </c>
-      <c r="D43" s="62">
+      <c r="D43" s="61">
         <v>207</v>
       </c>
       <c r="E43" s="13"/>
@@ -18810,10 +18840,10 @@
       <c r="B44" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C44" s="62">
+      <c r="C44" s="61">
         <v>212</v>
       </c>
-      <c r="D44" s="62">
+      <c r="D44" s="61">
         <v>223</v>
       </c>
       <c r="E44" s="13"/>
@@ -18825,10 +18855,10 @@
       <c r="B45" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="62">
+      <c r="C45" s="61">
         <v>228</v>
       </c>
-      <c r="D45" s="63">
+      <c r="D45" s="62">
         <v>239</v>
       </c>
       <c r="E45" s="13"/>
@@ -18840,10 +18870,10 @@
       <c r="B46" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C46" s="62">
+      <c r="C46" s="61">
         <v>244</v>
       </c>
-      <c r="D46" s="62">
+      <c r="D46" s="61">
         <v>255</v>
       </c>
       <c r="E46" s="13"/>
@@ -18855,10 +18885,10 @@
       <c r="B47" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C47" s="62">
+      <c r="C47" s="61">
         <v>260</v>
       </c>
-      <c r="D47" s="63">
+      <c r="D47" s="62">
         <v>271</v>
       </c>
       <c r="E47" s="13"/>
@@ -18870,10 +18900,10 @@
       <c r="B48" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C48" s="62">
+      <c r="C48" s="61">
         <v>276</v>
       </c>
-      <c r="D48" s="63">
+      <c r="D48" s="62">
         <v>287</v>
       </c>
       <c r="E48" s="13"/>
@@ -18885,10 +18915,10 @@
       <c r="B49" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C49" s="62">
+      <c r="C49" s="61">
         <v>292</v>
       </c>
-      <c r="D49" s="63">
+      <c r="D49" s="62">
         <v>303</v>
       </c>
       <c r="E49" s="13"/>
@@ -18900,10 +18930,10 @@
       <c r="B50" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C50" s="62">
+      <c r="C50" s="61">
         <v>308</v>
       </c>
-      <c r="D50" s="63">
+      <c r="D50" s="62">
         <v>319</v>
       </c>
       <c r="E50" s="13"/>
@@ -18918,7 +18948,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -18933,41 +18963,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="66"/>
+      <c r="C1" s="65"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="66"/>
+      <c r="C2" s="65"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="66" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="66"/>
+      <c r="C3" s="65"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A4" s="69"/>
-      <c r="B4" s="69"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>

</xml_diff>